<commit_message>
Update Customer B2C datasets in prep for v5.2. Incomplete changes
</commit_message>
<xml_diff>
--- a/demo-applications/customer-b2c/datasets/start-3-Products.xlsx
+++ b/demo-applications/customer-b2c/datasets/start-3-Products.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="29005"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdahlman/Google Drive/Semarchy WW/Customer Success/Getting Started Guide/Customer B2C/deliverables/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/semarchy/semarchy-git/xdm-tutorials/demo-applications/customer-b2c/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAE6746-C29A-4145-84B9-604C2A018E26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="460" windowWidth="25040" windowHeight="14500"/>
+    <workbookView xWindow="-33760" yWindow="3020" windowWidth="25040" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,11 +20,11 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -56,12 +57,6 @@
     <t>USA</t>
   </si>
   <si>
-    <t xml:space="preserve">Streamliner Roadster </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carbonite Century </t>
-  </si>
-  <si>
     <t xml:space="preserve">Full carbon aerodynamic road bike with extra durable frame. Ultra lightweight. Disc brakes and mechanical shifting. </t>
   </si>
   <si>
@@ -126,12 +121,18 @@
   </si>
   <si>
     <t>RENAUD4061LK</t>
+  </si>
+  <si>
+    <t>Streamliner Roadster</t>
+  </si>
+  <si>
+    <t>Carbonite Century</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -486,11 +487,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,12 +517,12 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -541,16 +542,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -561,13 +562,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -581,16 +582,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -601,16 +602,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -621,16 +622,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -641,16 +642,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
       </c>
       <c r="E8">
         <v>1</v>

</xml_diff>